<commit_message>
Changes related to making patterns user-defined. Minor renamings and edits. Drawings to paper checked in
</commit_message>
<xml_diff>
--- a/media/spreadsheets/Entropy.xlsx
+++ b/media/spreadsheets/Entropy.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>K=</t>
   </si>
@@ -53,18 +53,31 @@
   <si>
     <t>E/log(cell)</t>
   </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>No Confl:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -178,6 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,11 +1187,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145815808"/>
-        <c:axId val="145686528"/>
+        <c:axId val="146875520"/>
+        <c:axId val="146877056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145815808"/>
+        <c:axId val="146875520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,7 +1200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145686528"/>
+        <c:crossAx val="146877056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1194,7 +1208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145686528"/>
+        <c:axId val="146877056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145815808"/>
+        <c:crossAx val="146875520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3264,10 +3278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD7"/>
+  <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3277,7 +3291,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2">
         <v>1</v>
@@ -3290,7 +3304,7 @@
       </c>
       <c r="G1">
         <f>SUM(A1:D1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1">
         <v>1</v>
@@ -3314,18 +3328,18 @@
         <v>0</v>
       </c>
       <c r="P1" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q1" t="s">
         <v>8</v>
       </c>
       <c r="R1">
         <f>SUM(I1:P1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="XFD1">
         <f>SUM(A1:XFC1)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
@@ -3356,7 +3370,7 @@
       </c>
       <c r="B3" s="5">
         <f>SUM(A1:D1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
@@ -3372,19 +3386,19 @@
     <row r="4" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f>A1/$B$3</f>
-        <v>0.4</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="B4" s="5">
         <f t="shared" ref="B4:D4" si="0">B1/$B$3</f>
-        <v>0.2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -3394,19 +3408,19 @@
       </c>
       <c r="I4" s="4">
         <f>I1/$R$1</f>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ref="J4:P4" si="1">J1/$R$1</f>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="M4" s="5">
         <f t="shared" si="1"/>
@@ -3422,7 +3436,7 @@
       </c>
       <c r="P4" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="Q4" t="s">
         <v>9</v>
@@ -3438,46 +3452,46 @@
     <row r="5" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f>IF(A4&gt;0,-LOG(A4,2),0)</f>
-        <v>1.3219280948873622</v>
+        <v>1.5849625007211563</v>
       </c>
       <c r="B5" s="5">
         <f t="shared" ref="B5:D5" si="2">IF(B4&gt;0,-LOG(B4,2),0)</f>
-        <v>2.3219280948873622</v>
+        <v>1.5849625007211563</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="2"/>
-        <v>2.3219280948873622</v>
+        <v>2.5849625007211561</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="2"/>
-        <v>2.3219280948873622</v>
+        <v>2.5849625007211561</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="G5">
         <f>SUM(A5:D5)</f>
-        <v>8.2877123795494487</v>
+        <v>8.3398500028846243</v>
       </c>
       <c r="H5">
         <f>G5/4</f>
-        <v>2.0719280948873622</v>
+        <v>2.0849625007211561</v>
       </c>
       <c r="I5" s="4">
         <f>IF(I4&gt;0,-LOG(I4,2),0)</f>
-        <v>2.3219280948873622</v>
+        <v>3</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:P5" si="3">IF(J4&gt;0,-LOG(J4,2),0)</f>
-        <v>2.3219280948873622</v>
+        <v>3</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="3"/>
-        <v>2.3219280948873622</v>
+        <v>3</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="3"/>
-        <v>1.3219280948873622</v>
+        <v>2</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" si="3"/>
@@ -3493,18 +3507,18 @@
       </c>
       <c r="P5" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4150374992788437</v>
       </c>
       <c r="Q5" t="s">
         <v>5</v>
       </c>
       <c r="R5">
         <f>SUM(I5:P5)</f>
-        <v>8.2877123795494487</v>
+        <v>12.415037499278844</v>
       </c>
       <c r="S5">
         <f>R5/8</f>
-        <v>1.0359640474436811</v>
+        <v>1.5518796874098555</v>
       </c>
     </row>
     <row r="6" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
@@ -3514,7 +3528,7 @@
       </c>
       <c r="B6" s="5">
         <f t="shared" ref="B6:P6" si="4">IF(B1&lt;&gt;0,(B1-1)/B1,0)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="4"/>
@@ -3560,11 +3574,11 @@
       </c>
       <c r="P6" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="R6">
         <f t="shared" ref="R6:R7" si="5">SUM(I6:P6)</f>
-        <v>0.5</v>
+        <v>1.1666666666666665</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>11</v>
@@ -3573,11 +3587,11 @@
     <row r="7" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f>A4*A6</f>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="B7" s="8">
         <f t="shared" ref="B7:D7" si="6">B4*B6</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C7" s="8">
         <f t="shared" si="6"/>
@@ -3592,11 +3606,11 @@
       </c>
       <c r="G7">
         <f>SUM(A7:D7)</f>
-        <v>0.2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H7">
         <f>G5/2</f>
-        <v>4.1438561897747244</v>
+        <v>4.1699250014423122</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" ref="I7:P7" si="7">I4*I6</f>
@@ -3612,7 +3626,7 @@
       </c>
       <c r="L7" s="8">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="M7" s="8">
         <f t="shared" si="7"/>
@@ -3628,19 +3642,328 @@
       </c>
       <c r="P7" s="9">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q7" t="s">
         <v>6</v>
       </c>
       <c r="R7">
         <f t="shared" si="5"/>
-        <v>0.2</v>
+        <v>0.375</v>
       </c>
       <c r="S7">
         <f>R5/3</f>
-        <v>2.7625707931831496</v>
-      </c>
+        <v>4.1383458330929477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12/SUM(12:12)</f>
+        <v>0.05</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:R13" si="8">B12/SUM(12:12)</f>
+        <v>0.05</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="8"/>
+        <v>0.1</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="8"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>IF(A12&lt;&gt;0,(A12-1)/A12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:R14" si="9">IF(B12&lt;&gt;0,(B12-1)/B12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A13*A14</f>
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:R15" si="10">B13*B14</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="10"/>
+        <v>0.05</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="10"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f>SUM(15:15)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <f>1-B17</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <f>SUM(12:12)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>